<commit_message>
SELENIUM-284: Add excel test data as DataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blagoda\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blagoda\Desktop\phptravels\phptravels\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6E7D81-69E9-4D1D-B59B-D3F8E02F6DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF03D9D-8FDF-4AA4-B165-F53FB7AE6C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>city</t>
   </si>
@@ -36,10 +36,13 @@
     <t>Dubai</t>
   </si>
   <si>
-    <t>xxx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">London </t>
+    <t>Jumeirah Beach Hotel</t>
+  </si>
+  <si>
+    <t>Grand Plaza Apartments</t>
+  </si>
+  <si>
+    <t>London</t>
   </si>
 </sst>
 </file>
@@ -360,12 +363,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -386,10 +389,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>